<commit_message>
report 年度指标增加 alpha 和 beta
</commit_message>
<xml_diff>
--- a/rqalpha/mod/rqalpha_mod_sys_analyser/report/templates/summary.xlsx
+++ b/rqalpha/mod/rqalpha_mod_sys_analyser/report/templates/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ricequant\rqalpha\rqalpha\mod\rqalpha_mod_sys_analyser\report\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC84B93-646C-4507-B620-055F52108B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DD12C8-EBB8-4C89-88FD-1F4BF1334802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-270" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44760" yWindow="3690" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概览" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="196">
   <si>
     <t>策略名称</t>
   </si>
@@ -634,6 +634,22 @@
   <si>
     <t>超额最大回撤（几何）</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#alpha#</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>#beta#</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿尔法</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>贝塔</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2698,20 +2714,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.625" style="2" customWidth="1"/>
-    <col min="2" max="16" width="24.625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="2"/>
+    <col min="2" max="18" width="24.625" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
         <v>104</v>
       </c>
@@ -2760,8 +2776,14 @@
       <c r="P1" s="21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q1" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>112</v>
       </c>
@@ -2809,6 +2831,12 @@
       </c>
       <c r="P2" s="17" t="s">
         <v>77</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>